<commit_message>
Data Driven framework Automation testing
</commit_message>
<xml_diff>
--- a/src/test/resources/saucedemo.xlsx
+++ b/src/test/resources/saucedemo.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karamjeet\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF497AF-B57E-49FF-A6A0-BD70E96DFC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF1E57F-B986-4E99-8817-D414D3FE017E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="0" windowWidth="15375" windowHeight="10920" xr2:uid="{4BF21D33-1CB5-4366-B326-3882DE94FB05}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4BF21D33-1CB5-4366-B326-3882DE94FB05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>standard_user</t>
   </si>
@@ -55,13 +56,22 @@
   </si>
   <si>
     <t>problem_user</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>admin@maxxmann.in</t>
+  </si>
+  <si>
+    <t>Partner Agency Admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +101,14 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -109,10 +127,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -122,8 +141,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87BDBE4-010D-4C24-958C-3512EC18AF15}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -486,4 +510,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9C5443-5EB1-434B-ACE4-2F9E0E6A5577}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F46C7BCB-FD8D-4C00-A80B-EDAC5436A9EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2006-Data Driven framework Automation testing
</commit_message>
<xml_diff>
--- a/src/test/resources/saucedemo.xlsx
+++ b/src/test/resources/saucedemo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karamjeet\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF1E57F-B986-4E99-8817-D414D3FE017E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE63E72-535C-412F-AFC1-B5E7A192761F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4BF21D33-1CB5-4366-B326-3882DE94FB05}"/>
+    <workbookView xWindow="4110" yWindow="0" windowWidth="15375" windowHeight="10920" activeTab="1" xr2:uid="{4BF21D33-1CB5-4366-B326-3882DE94FB05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>